<commit_message>
complate!!-> scrapping whole ipl
</commit_message>
<xml_diff>
--- a/02_NodeJs/04_Web_Scrapping/02_Scrapping_IPL/ipl/Chennai Super Kings/Batting/Ambati Rayudu.xlsx
+++ b/02_NodeJs/04_Web_Scrapping/02_Scrapping_IPL/ipl/Chennai Super Kings/Batting/Ambati Rayudu.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ambati Rayudu" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,90 +397,588 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>matchNo</v>
+      </c>
+      <c r="B1" t="str">
         <v>teamName</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>batterName</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>states</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>runs</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>balls</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>fours</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>sixes</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>sr</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>opponentTeamName</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>venue</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>date</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>result</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Chennai Super Kings</v>
+        <v>53rd</v>
       </c>
       <c r="B2" t="str">
-        <v>Ambati Rayudu</v>
+        <v>Chennai Super Kings</v>
       </c>
       <c r="C2" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D2" t="str">
+        <v>c Arshdeep Singh b Jordan</v>
+      </c>
+      <c r="E2" t="str">
+        <v>4</v>
+      </c>
+      <c r="F2" t="str">
+        <v>5</v>
+      </c>
+      <c r="G2" t="str">
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <v>0</v>
+      </c>
+      <c r="I2" t="str">
+        <v>80.00</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Punjab Kings</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Dubai (DSC)</v>
+      </c>
+      <c r="L2" t="str">
+        <v>October 07</v>
+      </c>
+      <c r="M2" t="str">
+        <v>Punjab Kings won by 6 wickets (with 42 balls remaining)</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>47th</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D3" t="str">
+        <v>c Phillips b Sakariya</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2</v>
+      </c>
+      <c r="F3" t="str">
+        <v>4</v>
+      </c>
+      <c r="G3" t="str">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <v>50.00</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Rajasthan Royals</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Abu Dhabi</v>
+      </c>
+      <c r="L3" t="str">
+        <v>October 02</v>
+      </c>
+      <c r="M3" t="str">
+        <v>Royals won by 7 wickets (with 15 balls remaining)</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>44th</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v>17</v>
+      </c>
+      <c r="F4" t="str">
+        <v>13</v>
+      </c>
+      <c r="G4" t="str">
+        <v>1</v>
+      </c>
+      <c r="H4" t="str">
+        <v>1</v>
+      </c>
+      <c r="I4" t="str">
+        <v>130.76</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Sunrisers Hyderabad</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Sharjah</v>
+      </c>
+      <c r="L4" t="str">
+        <v>September 30</v>
+      </c>
+      <c r="M4" t="str">
+        <v>Super Kings won by 6 wickets (with 2 balls remaining)</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>50th</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v>55</v>
+      </c>
+      <c r="F5" t="str">
+        <v>43</v>
+      </c>
+      <c r="G5" t="str">
+        <v>5</v>
+      </c>
+      <c r="H5" t="str">
+        <v>2</v>
+      </c>
+      <c r="I5" t="str">
+        <v>127.90</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Dubai (DSC)</v>
+      </c>
+      <c r="L5" t="str">
+        <v>October 04</v>
+      </c>
+      <c r="M5" t="str">
+        <v>Capitals won by 3 wickets (with 2 balls remaining)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2nd</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D6" t="str">
+        <v>c Dhawan b Curran</v>
+      </c>
+      <c r="E6" t="str">
+        <v>23</v>
+      </c>
+      <c r="F6" t="str">
+        <v>16</v>
+      </c>
+      <c r="G6" t="str">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <v>2</v>
+      </c>
+      <c r="I6" t="str">
+        <v>143.75</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Wankhede</v>
+      </c>
+      <c r="L6" t="str">
+        <v>April 10</v>
+      </c>
+      <c r="M6" t="str">
+        <v>Capitals won by 7 wickets (with 8 balls remaining)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>8th</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D7" t="str">
+        <v>c Pooran b Mohammed Shami</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <v>0</v>
+      </c>
+      <c r="I7" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Punjab Kings</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Wankhede</v>
+      </c>
+      <c r="L7" t="str">
+        <v>April 16</v>
+      </c>
+      <c r="M7" t="str">
+        <v>Super Kings won by 6 wickets (with 26 balls remaining)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Qualifier</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D8" t="str">
         <v>run out (Iyer/Rabada)</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E8" t="str">
         <v>1</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F8" t="str">
         <v>3</v>
       </c>
-      <c r="F2" t="str">
-        <v>0</v>
-      </c>
-      <c r="G2" t="str">
-        <v>0</v>
-      </c>
-      <c r="H2" t="str">
+      <c r="G8" t="str">
+        <v>0</v>
+      </c>
+      <c r="H8" t="str">
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
         <v>33.33</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J8" t="str">
         <v>Delhi Capitals</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K8" t="str">
         <v>Dubai (DSC)</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L8" t="str">
         <v>October 10</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M8" t="str">
         <v>Super Kings won by 4 wickets (with 2 balls remaining)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>19th</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D9" t="str">
+        <v>c Jamieson b Patel</v>
+      </c>
+      <c r="E9" t="str">
+        <v>14</v>
+      </c>
+      <c r="F9" t="str">
+        <v>7</v>
+      </c>
+      <c r="G9" t="str">
+        <v>1</v>
+      </c>
+      <c r="H9" t="str">
+        <v>1</v>
+      </c>
+      <c r="I9" t="str">
+        <v>200.00</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Royal Challengers Bangalore</v>
+      </c>
+      <c r="K9" t="str">
+        <v>Wankhede</v>
+      </c>
+      <c r="L9" t="str">
+        <v>April 25</v>
+      </c>
+      <c r="M9" t="str">
+        <v>Super Kings won by 69 runs</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>27th</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <v>72</v>
+      </c>
+      <c r="F10" t="str">
+        <v>27</v>
+      </c>
+      <c r="G10" t="str">
+        <v>4</v>
+      </c>
+      <c r="H10" t="str">
+        <v>7</v>
+      </c>
+      <c r="I10" t="str">
+        <v>266.66</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="K10" t="str">
+        <v>Delhi</v>
+      </c>
+      <c r="L10" t="str">
+        <v>May 01</v>
+      </c>
+      <c r="M10" t="str">
+        <v>Mumbai won by 4 wickets</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>35th</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D11" t="str">
+        <v>c de Villiers b Patel</v>
+      </c>
+      <c r="E11" t="str">
+        <v>32</v>
+      </c>
+      <c r="F11" t="str">
+        <v>22</v>
+      </c>
+      <c r="G11" t="str">
+        <v>3</v>
+      </c>
+      <c r="H11" t="str">
+        <v>1</v>
+      </c>
+      <c r="I11" t="str">
+        <v>145.45</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Royal Challengers Bangalore</v>
+      </c>
+      <c r="K11" t="str">
+        <v>Sharjah</v>
+      </c>
+      <c r="L11" t="str">
+        <v>September 24</v>
+      </c>
+      <c r="M11" t="str">
+        <v>Super Kings won by 6 wickets (with 11 balls remaining)</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>30th</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
+        <v>3</v>
+      </c>
+      <c r="G12" t="str">
+        <v>0</v>
+      </c>
+      <c r="H12" t="str">
+        <v>0</v>
+      </c>
+      <c r="I12" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="K12" t="str">
+        <v>Dubai (DSC)</v>
+      </c>
+      <c r="L12" t="str">
+        <v>September 19</v>
+      </c>
+      <c r="M12" t="str">
+        <v>Super Kings won by 20 runs</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>38th</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D13" t="str">
+        <v>b Narine</v>
+      </c>
+      <c r="E13" t="str">
+        <v>10</v>
+      </c>
+      <c r="F13" t="str">
+        <v>9</v>
+      </c>
+      <c r="G13" t="str">
+        <v>1</v>
+      </c>
+      <c r="H13" t="str">
+        <v>0</v>
+      </c>
+      <c r="I13" t="str">
+        <v>111.11</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Kolkata Knight Riders</v>
+      </c>
+      <c r="K13" t="str">
+        <v>Abu Dhabi</v>
+      </c>
+      <c r="L13" t="str">
+        <v>September 26</v>
+      </c>
+      <c r="M13" t="str">
+        <v>Super Kings won by 2 wickets</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>12th</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Ambati Rayudu</v>
+      </c>
+      <c r="D14" t="str">
+        <v>c Parag b Sakariya</v>
+      </c>
+      <c r="E14" t="str">
+        <v>27</v>
+      </c>
+      <c r="F14" t="str">
+        <v>17</v>
+      </c>
+      <c r="G14" t="str">
+        <v>0</v>
+      </c>
+      <c r="H14" t="str">
+        <v>3</v>
+      </c>
+      <c r="I14" t="str">
+        <v>158.82</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Rajasthan Royals</v>
+      </c>
+      <c r="K14" t="str">
+        <v>Wankhede</v>
+      </c>
+      <c r="L14" t="str">
+        <v>April 19</v>
+      </c>
+      <c r="M14" t="str">
+        <v>Super Kings won by 45 runs</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>